<commit_message>
nuove attività e chiuse quelle vecchie
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/SpecificheIndicatori/Attivita.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/SpecificheIndicatori/Attivita.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\SpecificheIndicatori\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando.monaco\Desktop\ISP\SorgentiGIT\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\SpecificheIndicatori\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$80</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="246">
   <si>
     <t>Verificare/Cambiare tutte le formule indeterminate</t>
   </si>
@@ -718,9 +719,6 @@
     <t>UAT</t>
   </si>
   <si>
-    <t>rinviata al 2017</t>
-  </si>
-  <si>
     <t>override NOPG</t>
   </si>
   <si>
@@ -736,12 +734,6 @@
     <t>entro 11/11 ci mandano dati (MOL e Null) - entro il 23/11 - rinviato al 13/01 l'UAT</t>
   </si>
   <si>
-    <t>4 indicatori e 4 BR - UAT entro il 07/12</t>
-  </si>
-  <si>
-    <t>rilascio del 16/12 - rinviato al 13/01</t>
-  </si>
-  <si>
     <t>Spostamento 2 Notizie Pregiudiziali dal colore del ROSSO al BLU SCURO</t>
   </si>
   <si>
@@ -785,12 +777,27 @@
   </si>
   <si>
     <t>STATO PROD</t>
+  </si>
+  <si>
+    <t>rilascio il 20/01</t>
+  </si>
+  <si>
+    <t>FM/MD</t>
+  </si>
+  <si>
+    <t>override ind.36</t>
+  </si>
+  <si>
+    <t>rilascio il 20/02</t>
+  </si>
+  <si>
+    <t>Finanziamenti esteri: inserimento floor per calcolo giorni scaduto su indicatori importo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1309,277 +1316,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2180,27 +1917,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE125"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AE127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="9.875" customWidth="1"/>
-    <col min="3" max="3" width="83.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9.8984375" customWidth="1"/>
+    <col min="3" max="3" width="83.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.09765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" style="6" customWidth="1"/>
     <col min="6" max="6" width="11" style="6" customWidth="1"/>
     <col min="7" max="7" width="16.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.75" style="6" customWidth="1"/>
-    <col min="9" max="9" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="73.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.69921875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>18</v>
@@ -2218,7 +1956,7 @@
         <v>220</v>
       </c>
       <c r="G1" s="71" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>17</v>
@@ -2230,7 +1968,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="7">
         <v>1</v>
@@ -2260,7 +1998,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="7">
         <f>+B2+1</f>
@@ -2292,10 +2030,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="7">
-        <f t="shared" ref="B4:B78" si="0">+B3+1</f>
+        <f t="shared" ref="B4:B79" si="0">+B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -2322,7 +2060,7 @@
       <c r="J4" s="8"/>
       <c r="AE4" s="9"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="7">
         <f t="shared" si="0"/>
@@ -2340,7 +2078,9 @@
       <c r="F5" s="13">
         <v>1</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
       <c r="H5" s="5">
         <v>2</v>
       </c>
@@ -2350,7 +2090,7 @@
       <c r="J5" s="8"/>
       <c r="AE5" s="9"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="7">
         <f t="shared" si="0"/>
@@ -2365,8 +2105,12 @@
       <c r="E6" s="13">
         <v>1</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="F6" s="13">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
       <c r="H6" s="5">
         <v>3</v>
       </c>
@@ -2374,10 +2118,10 @@
         <v>3</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="7">
         <f t="shared" si="0"/>
@@ -2406,7 +2150,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="7">
         <f t="shared" si="0"/>
@@ -2435,7 +2179,7 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="7">
         <f t="shared" si="0"/>
@@ -2464,7 +2208,7 @@
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="7">
         <f t="shared" si="0"/>
@@ -2493,7 +2237,7 @@
       </c>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="7">
         <f t="shared" si="0"/>
@@ -2522,7 +2266,7 @@
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="7">
         <f t="shared" si="0"/>
@@ -2553,7 +2297,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="7">
         <f t="shared" si="0"/>
@@ -2582,7 +2326,7 @@
       </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="7">
         <f t="shared" si="0"/>
@@ -2611,7 +2355,7 @@
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="7">
         <f t="shared" si="0"/>
@@ -2640,7 +2384,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="7">
         <f t="shared" si="0"/>
@@ -2669,7 +2413,7 @@
       </c>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="7">
         <f t="shared" si="0"/>
@@ -2700,7 +2444,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="7">
         <f t="shared" si="0"/>
@@ -2729,7 +2473,7 @@
       </c>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="7">
         <f t="shared" si="0"/>
@@ -2758,7 +2502,7 @@
       </c>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="7">
         <f t="shared" si="0"/>
@@ -2789,7 +2533,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="7">
         <f t="shared" si="0"/>
@@ -2818,7 +2562,7 @@
       </c>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="7">
         <f t="shared" si="0"/>
@@ -2847,7 +2591,7 @@
       </c>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="7">
         <f t="shared" si="0"/>
@@ -2876,7 +2620,7 @@
       </c>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="7">
         <f t="shared" si="0"/>
@@ -2905,7 +2649,7 @@
       </c>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="7">
         <f t="shared" si="0"/>
@@ -2934,7 +2678,7 @@
       </c>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="7">
         <f t="shared" si="0"/>
@@ -2963,7 +2707,7 @@
       </c>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="7">
         <f t="shared" si="0"/>
@@ -2992,7 +2736,7 @@
       </c>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="7">
         <f t="shared" si="0"/>
@@ -3021,7 +2765,7 @@
       </c>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="7">
         <f t="shared" si="0"/>
@@ -3050,7 +2794,7 @@
       </c>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="7">
         <f t="shared" si="0"/>
@@ -3079,7 +2823,7 @@
       </c>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="7">
         <f t="shared" si="0"/>
@@ -3108,7 +2852,7 @@
       </c>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="7">
         <f t="shared" si="0"/>
@@ -3139,7 +2883,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="7">
         <f t="shared" si="0"/>
@@ -3168,7 +2912,7 @@
       </c>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="7">
         <f t="shared" si="0"/>
@@ -3197,7 +2941,7 @@
       </c>
       <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="7">
         <f t="shared" si="0"/>
@@ -3226,7 +2970,7 @@
       </c>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="7">
         <f t="shared" si="0"/>
@@ -3255,7 +2999,7 @@
       </c>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="7">
         <f t="shared" si="0"/>
@@ -3284,7 +3028,7 @@
       </c>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="7">
         <f t="shared" si="0"/>
@@ -3313,7 +3057,7 @@
       </c>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="7">
         <f t="shared" si="0"/>
@@ -3342,7 +3086,7 @@
       </c>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="7">
         <f t="shared" si="0"/>
@@ -3371,7 +3115,7 @@
       </c>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="7">
         <f t="shared" si="0"/>
@@ -3402,7 +3146,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="7">
         <f t="shared" si="0"/>
@@ -3431,7 +3175,7 @@
       </c>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="7">
         <f t="shared" si="0"/>
@@ -3462,7 +3206,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="7">
         <f t="shared" si="0"/>
@@ -3493,7 +3237,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="7">
         <f t="shared" si="0"/>
@@ -3508,8 +3252,12 @@
       <c r="E45" s="13">
         <v>1</v>
       </c>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
+      <c r="F45" s="13">
+        <v>1</v>
+      </c>
+      <c r="G45" s="13">
+        <v>1</v>
+      </c>
       <c r="H45" s="5">
         <v>3</v>
       </c>
@@ -3517,10 +3265,10 @@
         <v>3</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="7">
         <f t="shared" si="0"/>
@@ -3551,7 +3299,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="7">
         <f t="shared" si="0"/>
@@ -3563,9 +3311,15 @@
       <c r="D47" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
+      <c r="E47" s="13">
+        <v>1</v>
+      </c>
+      <c r="F47" s="13">
+        <v>0</v>
+      </c>
+      <c r="G47" s="13">
+        <v>0</v>
+      </c>
       <c r="H47" s="5">
         <v>2</v>
       </c>
@@ -3573,10 +3327,10 @@
         <v>1</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="7">
         <f t="shared" si="0"/>
@@ -3588,9 +3342,7 @@
       <c r="D48" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E48" s="13" t="s">
-        <v>173</v>
-      </c>
+      <c r="E48" s="13"/>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="5">
@@ -3599,7 +3351,7 @@
       <c r="I48" s="5"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="7">
         <f t="shared" si="0"/>
@@ -3630,7 +3382,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="7">
         <f t="shared" si="0"/>
@@ -3661,7 +3413,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="7">
         <f t="shared" si="0"/>
@@ -3692,7 +3444,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B52" s="7">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -3722,7 +3474,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B53" s="7">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -3739,7 +3491,9 @@
       <c r="F53" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G53" s="13"/>
+      <c r="G53" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="H53" s="5">
         <v>1</v>
       </c>
@@ -3750,7 +3504,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B54" s="7">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -3761,9 +3515,7 @@
       <c r="D54" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="13" t="s">
-        <v>173</v>
-      </c>
+      <c r="E54" s="13"/>
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
       <c r="H54" s="5">
@@ -3776,7 +3528,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B55" s="7">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -3785,10 +3537,10 @@
         <v>182</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E55" s="13" t="s">
-        <v>173</v>
+        <v>242</v>
+      </c>
+      <c r="E55" s="13">
+        <v>0.15</v>
       </c>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
@@ -3799,10 +3551,10 @@
         <v>3</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B56" s="7">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -3832,7 +3584,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B57" s="7">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -3862,7 +3614,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B58" s="7">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -3888,7 +3640,7 @@
       </c>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B59" s="7">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -3914,7 +3666,7 @@
       </c>
       <c r="J59" s="1"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B60" s="7">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -3940,7 +3692,7 @@
       </c>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B61" s="7">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -3970,7 +3722,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B62" s="7">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -3996,7 +3748,7 @@
       </c>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B63" s="7">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -4013,7 +3765,9 @@
       <c r="F63" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G63" s="13"/>
+      <c r="G63" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="H63" s="5">
         <v>3</v>
       </c>
@@ -4022,7 +3776,7 @@
       </c>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B64" s="7">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -4039,7 +3793,9 @@
       <c r="F64" s="13">
         <v>1</v>
       </c>
-      <c r="G64" s="13"/>
+      <c r="G64" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="H64" s="5">
         <v>1</v>
       </c>
@@ -4050,7 +3806,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B65" s="7">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -4080,7 +3836,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B66" s="7">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -4106,7 +3862,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B67" s="7">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -4130,7 +3886,7 @@
       </c>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B68" s="7">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -4147,7 +3903,9 @@
       <c r="F68" s="13">
         <v>1</v>
       </c>
-      <c r="G68" s="13"/>
+      <c r="G68" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="H68" s="5">
         <v>1</v>
       </c>
@@ -4156,7 +3914,7 @@
       </c>
       <c r="J68" s="1"/>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B69" s="7">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -4173,7 +3931,9 @@
       <c r="F69" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G69" s="13"/>
+      <c r="G69" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="H69" s="5">
         <v>1</v>
       </c>
@@ -4182,7 +3942,7 @@
       </c>
       <c r="J69" s="1"/>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B70" s="7">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -4191,9 +3951,11 @@
         <v>219</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E70" s="13"/>
+        <v>242</v>
+      </c>
+      <c r="E70" s="13">
+        <v>0.15</v>
+      </c>
       <c r="F70" s="13"/>
       <c r="G70" s="13"/>
       <c r="H70" s="5">
@@ -4203,21 +3965,23 @@
         <v>3</v>
       </c>
       <c r="J70" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B71" s="7">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" s="7">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>222</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E71" s="13"/>
+      <c r="E71" s="13">
+        <v>0.15</v>
+      </c>
       <c r="F71" s="13"/>
       <c r="G71" s="13"/>
       <c r="H71" s="5">
@@ -4227,23 +3991,29 @@
         <v>2</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="B72" s="7">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
+      <c r="E72" s="13">
+        <v>1</v>
+      </c>
+      <c r="F72" s="13">
+        <v>1</v>
+      </c>
+      <c r="G72" s="13">
+        <v>1</v>
+      </c>
       <c r="H72" s="5">
         <v>1</v>
       </c>
@@ -4251,23 +4021,29 @@
         <v>1</v>
       </c>
       <c r="J72" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="7">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="C73" s="10" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" s="7">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>224</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
+      <c r="E73" s="13">
+        <v>1</v>
+      </c>
+      <c r="F73" s="13">
+        <v>1</v>
+      </c>
+      <c r="G73" s="13">
+        <v>1</v>
+      </c>
       <c r="H73" s="5">
         <v>1</v>
       </c>
@@ -4275,22 +4051,22 @@
         <v>1</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B74" s="7">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D74" s="70" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F74" s="13"/>
       <c r="G74" s="13"/>
@@ -4301,16 +4077,16 @@
         <v>1</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B75" s="7">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D75" s="70" t="s">
         <v>24</v>
@@ -4325,16 +4101,16 @@
         <v>1</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B76" s="7">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D76" s="70" t="s">
         <v>24</v>
@@ -4350,16 +4126,16 @@
       </c>
       <c r="J76" s="1"/>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B77" s="7">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D77" s="70" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E77" s="13"/>
       <c r="F77" s="13" t="s">
@@ -4373,16 +4149,16 @@
         <v>2</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B78" s="7">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D78" s="70" t="s">
         <v>25</v>
@@ -4397,65 +4173,87 @@
         <v>3</v>
       </c>
       <c r="J78" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B79" s="7">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="D79" s="70" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
+      <c r="E79" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="5">
+        <v>2</v>
+      </c>
+      <c r="I79" s="5">
+        <v>1</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B80" s="7">
+        <f>+B79+1</f>
+        <v>79</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D80" s="70" t="s">
+        <v>242</v>
+      </c>
+      <c r="E80" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="5">
+        <v>3</v>
+      </c>
+      <c r="I80" s="5">
+        <v>2</v>
+      </c>
+      <c r="J80" s="1"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
         <v>210</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D82" s="6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="69">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B83" s="69">
         <v>42668</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C83" t="s">
         <v>197</v>
       </c>
-      <c r="D81" s="68">
+      <c r="D83" s="68">
         <v>42678</v>
       </c>
-      <c r="E81" s="6" t="s">
+      <c r="E83" s="6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="69">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B84" s="69">
         <v>42669</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C84" t="s">
         <v>198</v>
-      </c>
-      <c r="D82" s="68">
-        <v>42691</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="69">
-        <v>42670</v>
-      </c>
-      <c r="C83" t="s">
-        <v>200</v>
-      </c>
-      <c r="D83" s="68">
-        <v>42691</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="67">
-        <v>42676</v>
-      </c>
-      <c r="C84" t="s">
-        <v>199</v>
       </c>
       <c r="D84" s="68">
         <v>42691</v>
@@ -4464,161 +4262,216 @@
         <v>216</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="67">
-        <v>42671</v>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B85" s="69">
+        <v>42670</v>
       </c>
       <c r="C85" t="s">
-        <v>201</v>
-      </c>
-      <c r="D85" s="68"/>
+        <v>200</v>
+      </c>
+      <c r="D85" s="68">
+        <v>42691</v>
+      </c>
       <c r="E85" s="6" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="69">
-        <v>42668</v>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B86" s="67">
+        <v>42676</v>
       </c>
       <c r="C86" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D86" s="68">
-        <v>42671</v>
+        <v>42691</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" t="s">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B87" s="67">
+        <v>42671</v>
+      </c>
+      <c r="C87" t="s">
+        <v>201</v>
+      </c>
+      <c r="D87" s="68"/>
+      <c r="E87" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B88" s="69">
+        <v>42668</v>
+      </c>
+      <c r="C88" t="s">
+        <v>202</v>
+      </c>
+      <c r="D88" s="68">
+        <v>42671</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J68"/>
+  <autoFilter ref="A1:J80">
+    <filterColumn colId="6">
+      <filters blank="1">
+        <filter val="0%"/>
+        <filter val="NO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="E1:G16 F2:G70 E18:G68">
-    <cfRule type="cellIs" dxfId="55" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:G17 G18:G44">
-    <cfRule type="cellIs" dxfId="54" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="31" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69:G69">
-    <cfRule type="cellIs" dxfId="53" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70:G70">
-    <cfRule type="cellIs" dxfId="52" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71:G71">
-    <cfRule type="cellIs" dxfId="51" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71:G71">
-    <cfRule type="cellIs" dxfId="50" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F72:G72">
-    <cfRule type="cellIs" dxfId="49" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E72:G72">
-    <cfRule type="cellIs" dxfId="48" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F73:G73">
-    <cfRule type="cellIs" dxfId="47" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73:G73">
-    <cfRule type="cellIs" dxfId="46" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F74:G74">
-    <cfRule type="cellIs" dxfId="45" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:G74">
-    <cfRule type="cellIs" dxfId="44" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F75:G75">
-    <cfRule type="cellIs" dxfId="43" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E75:G75">
-    <cfRule type="cellIs" dxfId="42" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F76:G76">
-    <cfRule type="cellIs" dxfId="41" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76:G76">
-    <cfRule type="cellIs" dxfId="40" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="39" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F77:G77">
-    <cfRule type="cellIs" dxfId="38" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77:G77">
-    <cfRule type="cellIs" dxfId="37" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F78:G78">
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:G78">
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51:G52">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G45">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F79:G80">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E79:G79 F80:G80">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E80">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4635,14 +4488,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.75" customWidth="1"/>
-    <col min="2" max="2" width="28.875" customWidth="1"/>
+    <col min="1" max="1" width="5.69921875" customWidth="1"/>
+    <col min="2" max="2" width="28.8984375" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>44</v>
       </c>
@@ -4650,7 +4503,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>41</v>
       </c>
@@ -4661,7 +4514,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -4672,7 +4525,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>43</v>
       </c>
@@ -4683,7 +4536,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>43</v>
       </c>
@@ -4694,7 +4547,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>43</v>
       </c>
@@ -4705,7 +4558,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>43</v>
       </c>
@@ -4716,7 +4569,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>43</v>
       </c>
@@ -4727,7 +4580,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>43</v>
       </c>
@@ -4738,7 +4591,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" t="s">
         <v>33</v>
@@ -4763,21 +4616,21 @@
       <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="2.75" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.125" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="2.69921875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.09765625" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="61" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.125" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.25" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.09765625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.19921875" style="27" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="9.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.25" style="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.75" style="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.75" style="27"/>
+    <col min="11" max="12" width="8.19921875" style="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.69921875" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.69921875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>170</v>
       </c>
@@ -4818,7 +4671,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28"/>
       <c r="B3" s="28">
         <v>23</v>
@@ -4853,7 +4706,7 @@
       <c r="L3" s="33"/>
       <c r="M3" s="23"/>
     </row>
-    <row r="4" spans="1:13" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>171</v>
       </c>
@@ -4892,7 +4745,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="38"/>
       <c r="B5" s="38"/>
       <c r="C5" s="39"/>
@@ -4915,7 +4768,7 @@
       <c r="L5" s="38"/>
       <c r="M5" s="25"/>
     </row>
-    <row r="6" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A6" s="34"/>
       <c r="B6" s="34">
         <v>3</v>
@@ -4950,7 +4803,7 @@
       <c r="L6" s="34"/>
       <c r="M6" s="24"/>
     </row>
-    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="38"/>
       <c r="B7" s="38"/>
       <c r="C7" s="44"/>
@@ -4967,7 +4820,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="25"/>
     </row>
-    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A8" s="34"/>
       <c r="B8" s="34">
         <v>4</v>
@@ -5002,7 +4855,7 @@
       <c r="L8" s="34"/>
       <c r="M8" s="24"/>
     </row>
-    <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
       <c r="C9" s="44"/>
@@ -5019,7 +4872,7 @@
       <c r="L9" s="38"/>
       <c r="M9" s="25"/>
     </row>
-    <row r="10" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="34"/>
       <c r="B10" s="34">
         <v>26</v>
@@ -5054,7 +4907,7 @@
       <c r="L10" s="34"/>
       <c r="M10" s="24"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="46"/>
       <c r="B11" s="46"/>
       <c r="C11" s="47"/>
@@ -5071,7 +4924,7 @@
       <c r="L11" s="46"/>
       <c r="M11" s="26"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="46"/>
       <c r="B12" s="46"/>
       <c r="C12" s="47"/>
@@ -5088,7 +4941,7 @@
       <c r="L12" s="46"/>
       <c r="M12" s="26"/>
     </row>
-    <row r="13" spans="1:13" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
       <c r="C13" s="39"/>
@@ -5105,7 +4958,7 @@
       <c r="L13" s="38"/>
       <c r="M13" s="25"/>
     </row>
-    <row r="14" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="34"/>
       <c r="B14" s="34">
         <v>2</v>
@@ -5140,7 +4993,7 @@
       <c r="L14" s="34"/>
       <c r="M14" s="24"/>
     </row>
-    <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="39"/>
@@ -5161,7 +5014,7 @@
       <c r="L15" s="38"/>
       <c r="M15" s="25"/>
     </row>
-    <row r="16" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28"/>
       <c r="B16" s="28">
         <v>24</v>
@@ -5198,7 +5051,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
         <v>171</v>
       </c>
@@ -5237,7 +5090,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="39"/>
@@ -5260,7 +5113,7 @@
       <c r="L18" s="38"/>
       <c r="M18" s="25"/>
     </row>
-    <row r="19" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="34"/>
       <c r="B19" s="34">
         <v>22</v>
@@ -5293,7 +5146,7 @@
       <c r="L19" s="34"/>
       <c r="M19" s="24"/>
     </row>
-    <row r="20" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="29" t="s">
@@ -5310,7 +5163,7 @@
       <c r="L20" s="38"/>
       <c r="M20" s="25"/>
     </row>
-    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A21" s="34"/>
       <c r="B21" s="34">
         <v>20</v>
@@ -5345,7 +5198,7 @@
       <c r="L21" s="34"/>
       <c r="M21" s="24"/>
     </row>
-    <row r="22" spans="1:13" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="38"/>
       <c r="B22" s="38"/>
       <c r="C22" s="39"/>
@@ -5362,7 +5215,7 @@
       <c r="L22" s="38"/>
       <c r="M22" s="25"/>
     </row>
-    <row r="23" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="34" t="s">
         <v>171</v>
       </c>
@@ -5401,7 +5254,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="46"/>
       <c r="B24" s="46"/>
       <c r="C24" s="47"/>
@@ -5426,7 +5279,7 @@
       <c r="L24" s="46"/>
       <c r="M24" s="26"/>
     </row>
-    <row r="25" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="46"/>
       <c r="B25" s="46"/>
       <c r="C25" s="47"/>
@@ -5443,7 +5296,7 @@
       <c r="L25" s="46"/>
       <c r="M25" s="26"/>
     </row>
-    <row r="26" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="46"/>
       <c r="B26" s="46"/>
       <c r="C26" s="47"/>
@@ -5460,7 +5313,7 @@
       <c r="L26" s="46"/>
       <c r="M26" s="26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="46"/>
       <c r="B27" s="46"/>
       <c r="C27" s="47"/>
@@ -5477,7 +5330,7 @@
       <c r="L27" s="46"/>
       <c r="M27" s="26"/>
     </row>
-    <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="38"/>
       <c r="B28" s="38"/>
       <c r="C28" s="39"/>
@@ -5494,7 +5347,7 @@
       <c r="L28" s="38"/>
       <c r="M28" s="25"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="34"/>
       <c r="B29" s="34">
         <v>7</v>
@@ -5529,7 +5382,7 @@
       <c r="L29" s="34"/>
       <c r="M29" s="24"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="46"/>
       <c r="B30" s="46"/>
       <c r="C30" s="47"/>
@@ -5546,7 +5399,7 @@
       <c r="L30" s="46"/>
       <c r="M30" s="26"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="46"/>
       <c r="B31" s="46"/>
       <c r="C31" s="47"/>
@@ -5563,7 +5416,7 @@
       <c r="L31" s="46"/>
       <c r="M31" s="26"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="46"/>
       <c r="B32" s="46"/>
       <c r="C32" s="47"/>
@@ -5580,7 +5433,7 @@
       <c r="L32" s="46"/>
       <c r="M32" s="26"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="46"/>
       <c r="B33" s="46"/>
       <c r="C33" s="47"/>
@@ -5597,7 +5450,7 @@
       <c r="L33" s="46"/>
       <c r="M33" s="26"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="46"/>
       <c r="B34" s="46"/>
       <c r="C34" s="47"/>
@@ -5614,7 +5467,7 @@
       <c r="L34" s="46"/>
       <c r="M34" s="26"/>
     </row>
-    <row r="35" spans="1:13" ht="68.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="38"/>
       <c r="B35" s="38"/>
       <c r="C35" s="39"/>
@@ -5631,7 +5484,7 @@
       <c r="L35" s="38"/>
       <c r="M35" s="25"/>
     </row>
-    <row r="36" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="28" t="s">
         <v>171</v>
       </c>
@@ -5670,7 +5523,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="34"/>
       <c r="B37" s="34">
         <v>9</v>
@@ -5705,7 +5558,7 @@
       <c r="L37" s="34"/>
       <c r="M37" s="24"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="46"/>
       <c r="B38" s="46"/>
       <c r="C38" s="47"/>
@@ -5722,7 +5575,7 @@
       <c r="L38" s="46"/>
       <c r="M38" s="26"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="46"/>
       <c r="B39" s="46"/>
       <c r="C39" s="47"/>
@@ -5739,7 +5592,7 @@
       <c r="L39" s="46"/>
       <c r="M39" s="26"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="46"/>
       <c r="B40" s="46"/>
       <c r="C40" s="47"/>
@@ -5756,7 +5609,7 @@
       <c r="L40" s="46"/>
       <c r="M40" s="26"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="46"/>
       <c r="B41" s="46"/>
       <c r="C41" s="47"/>
@@ -5773,7 +5626,7 @@
       <c r="L41" s="46"/>
       <c r="M41" s="26"/>
     </row>
-    <row r="42" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="38"/>
       <c r="B42" s="38"/>
       <c r="C42" s="39"/>
@@ -5790,7 +5643,7 @@
       <c r="L42" s="38"/>
       <c r="M42" s="25"/>
     </row>
-    <row r="43" spans="1:13" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="28"/>
       <c r="B43" s="28">
         <v>10</v>
@@ -5825,7 +5678,7 @@
       <c r="L43" s="33"/>
       <c r="M43" s="23"/>
     </row>
-    <row r="44" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="41.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="28"/>
       <c r="B44" s="28">
         <v>16</v>

</xml_diff>

<commit_message>
update e caricamento file vecchi salvati sul mio deck
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/SpecificheIndicatori/Attivita.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/SpecificheIndicatori/Attivita.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="265">
   <si>
     <t>Verificare/Cambiare tutte le formule indeterminate</t>
   </si>
@@ -1021,6 +1021,33 @@
   </si>
   <si>
     <t>dati/output</t>
+  </si>
+  <si>
+    <t>fine sviluppi</t>
+  </si>
+  <si>
+    <t>fine test</t>
+  </si>
+  <si>
+    <t>apertura UDC</t>
+  </si>
+  <si>
+    <t>campi ETL in test</t>
+  </si>
+  <si>
+    <t>campi ETL in dev</t>
+  </si>
+  <si>
+    <t>chiusura UDC o UDE</t>
+  </si>
+  <si>
+    <t>go-live</t>
+  </si>
+  <si>
+    <t>intervento correttivo XRA</t>
+  </si>
+  <si>
+    <t>FM/MD/MC</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1471,11 +1498,72 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="133">
+  <dxfs count="139">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3122,10 +3210,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AE128"/>
+  <dimension ref="A1:AE129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -5512,7 +5600,7 @@
         <v>132</v>
       </c>
       <c r="E83" s="13">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="F83" s="13"/>
       <c r="G83" s="13"/>
@@ -5538,7 +5626,7 @@
         <v>132</v>
       </c>
       <c r="E84" s="13">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F84" s="13"/>
       <c r="G84" s="13"/>
@@ -5962,7 +6050,7 @@
     </row>
     <row r="101" spans="2:10">
       <c r="B101" s="7">
-        <f t="shared" ref="B101:B121" si="4">+B100+1</f>
+        <f t="shared" ref="B101:B122" si="4">+B100+1</f>
         <v>100</v>
       </c>
       <c r="C101" s="10" t="s">
@@ -6190,7 +6278,7 @@
         <v>25</v>
       </c>
       <c r="E110" s="13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F110" s="13"/>
       <c r="G110" s="13"/>
@@ -6469,39 +6557,61 @@
       </c>
     </row>
     <row r="122" spans="2:10">
-      <c r="D122"/>
-      <c r="E122"/>
-      <c r="F122"/>
-      <c r="G122"/>
-      <c r="H122"/>
+      <c r="B122" s="7">
+        <f t="shared" si="4"/>
+        <v>121</v>
+      </c>
+      <c r="C122" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="D122" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="E122" s="13"/>
+      <c r="F122" s="13"/>
+      <c r="G122" s="13"/>
+      <c r="H122" s="5">
+        <v>1</v>
+      </c>
+      <c r="I122" s="5">
+        <v>2</v>
+      </c>
+      <c r="J122" s="1"/>
     </row>
     <row r="123" spans="2:10">
-      <c r="C123" s="31" t="s">
-        <v>165</v>
-      </c>
+      <c r="D123"/>
+      <c r="E123"/>
+      <c r="F123"/>
+      <c r="G123"/>
+      <c r="H123"/>
     </row>
     <row r="124" spans="2:10">
       <c r="C124" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="125" spans="2:10">
       <c r="C125" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="126" spans="2:10">
       <c r="C126" s="31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="127" spans="2:10">
+      <c r="C127" s="31" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="127" spans="2:10">
-      <c r="C127" s="38" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="128" spans="2:10">
       <c r="C128" s="38" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3">
+      <c r="C129" s="38" t="s">
         <v>202</v>
       </c>
     </row>
@@ -6512,667 +6622,682 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="E1:G16 F2:G70 E18:G68">
+    <cfRule type="cellIs" dxfId="138" priority="151" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:G17 G18:G44">
+    <cfRule type="cellIs" dxfId="137" priority="150" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69:G69">
+    <cfRule type="cellIs" dxfId="136" priority="149" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70:G70">
+    <cfRule type="cellIs" dxfId="135" priority="148" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F71:G71">
+    <cfRule type="cellIs" dxfId="134" priority="147" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71:G71">
+    <cfRule type="cellIs" dxfId="133" priority="146" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F72:G72">
     <cfRule type="cellIs" dxfId="132" priority="145" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:G17 G18:G44">
+  <conditionalFormatting sqref="E72:G72">
     <cfRule type="cellIs" dxfId="131" priority="144" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69:G69">
+  <conditionalFormatting sqref="F73:G73">
     <cfRule type="cellIs" dxfId="130" priority="143" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E70:G70">
+  <conditionalFormatting sqref="E73:G73">
     <cfRule type="cellIs" dxfId="129" priority="142" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F71:G71">
+  <conditionalFormatting sqref="F74:G74">
     <cfRule type="cellIs" dxfId="128" priority="141" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E71:G71">
+  <conditionalFormatting sqref="E74:G74">
     <cfRule type="cellIs" dxfId="127" priority="140" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F72:G72">
+  <conditionalFormatting sqref="F75:G75">
     <cfRule type="cellIs" dxfId="126" priority="139" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E72:G72">
+  <conditionalFormatting sqref="E75:G75">
     <cfRule type="cellIs" dxfId="125" priority="138" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F73:G73">
+  <conditionalFormatting sqref="F76:G76">
     <cfRule type="cellIs" dxfId="124" priority="137" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73:G73">
+  <conditionalFormatting sqref="E76:G76">
     <cfRule type="cellIs" dxfId="123" priority="136" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F74:G74">
+  <conditionalFormatting sqref="E69">
     <cfRule type="cellIs" dxfId="122" priority="135" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74:G74">
+  <conditionalFormatting sqref="F77:G77">
     <cfRule type="cellIs" dxfId="121" priority="134" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F75:G75">
+  <conditionalFormatting sqref="E77:G77">
     <cfRule type="cellIs" dxfId="120" priority="133" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E75:G75">
+  <conditionalFormatting sqref="F78:G78">
     <cfRule type="cellIs" dxfId="119" priority="132" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F76:G76">
+  <conditionalFormatting sqref="E78:G78">
     <cfRule type="cellIs" dxfId="118" priority="131" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E76:G76">
+  <conditionalFormatting sqref="G46">
     <cfRule type="cellIs" dxfId="117" priority="130" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+  <conditionalFormatting sqref="G49">
     <cfRule type="cellIs" dxfId="116" priority="129" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F77:G77">
+  <conditionalFormatting sqref="G50">
     <cfRule type="cellIs" dxfId="115" priority="128" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E77:G77">
+  <conditionalFormatting sqref="G51:G52">
     <cfRule type="cellIs" dxfId="114" priority="127" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F78:G78">
+  <conditionalFormatting sqref="G45">
     <cfRule type="cellIs" dxfId="113" priority="126" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E78:G78">
+  <conditionalFormatting sqref="F79:G80">
     <cfRule type="cellIs" dxfId="112" priority="125" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
+  <conditionalFormatting sqref="E79:G79 F80:G80">
     <cfRule type="cellIs" dxfId="111" priority="124" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
+  <conditionalFormatting sqref="E80">
     <cfRule type="cellIs" dxfId="110" priority="123" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G50">
-    <cfRule type="cellIs" dxfId="109" priority="122" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G51:G52">
-    <cfRule type="cellIs" dxfId="108" priority="121" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="cellIs" dxfId="107" priority="120" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F79:G80">
-    <cfRule type="cellIs" dxfId="106" priority="119" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E79:G79 F80:G80">
-    <cfRule type="cellIs" dxfId="105" priority="118" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E80">
-    <cfRule type="cellIs" dxfId="104" priority="117" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F81:G82">
+    <cfRule type="cellIs" dxfId="109" priority="119" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F81:G82">
+    <cfRule type="cellIs" dxfId="108" priority="118" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E81:E82">
+    <cfRule type="cellIs" dxfId="107" priority="117" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F83:G83">
+    <cfRule type="cellIs" dxfId="106" priority="116" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F83:G83">
+    <cfRule type="cellIs" dxfId="105" priority="115" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E83">
+    <cfRule type="cellIs" dxfId="104" priority="114" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F84:G84">
     <cfRule type="cellIs" dxfId="103" priority="113" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F81:G82">
+  <conditionalFormatting sqref="F84:G84">
     <cfRule type="cellIs" dxfId="102" priority="112" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E81:E82">
+  <conditionalFormatting sqref="E84">
     <cfRule type="cellIs" dxfId="101" priority="111" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F83:G83">
+  <conditionalFormatting sqref="F86:G86">
     <cfRule type="cellIs" dxfId="100" priority="110" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F83:G83">
+  <conditionalFormatting sqref="F86:G86">
     <cfRule type="cellIs" dxfId="99" priority="109" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E83">
+  <conditionalFormatting sqref="E86">
     <cfRule type="cellIs" dxfId="98" priority="108" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F84:G84">
+  <conditionalFormatting sqref="F87:G87">
     <cfRule type="cellIs" dxfId="97" priority="107" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F84:G84">
+  <conditionalFormatting sqref="F87:G87">
     <cfRule type="cellIs" dxfId="96" priority="106" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+  <conditionalFormatting sqref="E87">
     <cfRule type="cellIs" dxfId="95" priority="105" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F86:G86">
+  <conditionalFormatting sqref="F85:G85">
     <cfRule type="cellIs" dxfId="94" priority="104" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F86:G86">
+  <conditionalFormatting sqref="F85:G85">
     <cfRule type="cellIs" dxfId="93" priority="103" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E86">
+  <conditionalFormatting sqref="E85">
     <cfRule type="cellIs" dxfId="92" priority="102" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F87:G87">
+  <conditionalFormatting sqref="F88:G88">
     <cfRule type="cellIs" dxfId="91" priority="101" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F87:G87">
+  <conditionalFormatting sqref="F88:G88">
     <cfRule type="cellIs" dxfId="90" priority="100" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
+  <conditionalFormatting sqref="E88">
     <cfRule type="cellIs" dxfId="89" priority="99" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F85:G85">
+  <conditionalFormatting sqref="F90:G90">
     <cfRule type="cellIs" dxfId="88" priority="98" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F85:G85">
+  <conditionalFormatting sqref="F90:G90">
     <cfRule type="cellIs" dxfId="87" priority="97" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85">
+  <conditionalFormatting sqref="E90">
     <cfRule type="cellIs" dxfId="86" priority="96" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F88:G88">
+  <conditionalFormatting sqref="F91:G91">
     <cfRule type="cellIs" dxfId="85" priority="95" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F88:G88">
+  <conditionalFormatting sqref="F91:G91">
     <cfRule type="cellIs" dxfId="84" priority="94" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E88">
+  <conditionalFormatting sqref="E91">
     <cfRule type="cellIs" dxfId="83" priority="93" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90:G90">
+  <conditionalFormatting sqref="F89">
     <cfRule type="cellIs" dxfId="82" priority="92" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90:G90">
+  <conditionalFormatting sqref="F89">
     <cfRule type="cellIs" dxfId="81" priority="91" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E90">
+  <conditionalFormatting sqref="E89">
     <cfRule type="cellIs" dxfId="80" priority="90" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F91:G91">
+  <conditionalFormatting sqref="F92:G92">
     <cfRule type="cellIs" dxfId="79" priority="89" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F91:G91">
+  <conditionalFormatting sqref="F92:G92">
     <cfRule type="cellIs" dxfId="78" priority="88" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E91">
+  <conditionalFormatting sqref="E92">
     <cfRule type="cellIs" dxfId="77" priority="87" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F89">
-    <cfRule type="cellIs" dxfId="76" priority="86" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F89">
-    <cfRule type="cellIs" dxfId="75" priority="85" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E89">
-    <cfRule type="cellIs" dxfId="74" priority="84" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F92:G92">
-    <cfRule type="cellIs" dxfId="73" priority="83" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F92:G92">
-    <cfRule type="cellIs" dxfId="72" priority="82" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="71" priority="81" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F93:G93">
+    <cfRule type="cellIs" dxfId="76" priority="80" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E93:G93">
+    <cfRule type="cellIs" dxfId="75" priority="79" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F94:G94">
+    <cfRule type="cellIs" dxfId="74" priority="78" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F94:G94">
+    <cfRule type="cellIs" dxfId="73" priority="77" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F95:G95">
+    <cfRule type="cellIs" dxfId="72" priority="76" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E95:G95">
+    <cfRule type="cellIs" dxfId="71" priority="75" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F96:G96">
     <cfRule type="cellIs" dxfId="70" priority="74" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E93:G93">
+  <conditionalFormatting sqref="F96:G96">
     <cfRule type="cellIs" dxfId="69" priority="73" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F94:G94">
+  <conditionalFormatting sqref="E94">
     <cfRule type="cellIs" dxfId="68" priority="72" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F94:G94">
+  <conditionalFormatting sqref="E96">
     <cfRule type="cellIs" dxfId="67" priority="71" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F95:G95">
+  <conditionalFormatting sqref="F97">
     <cfRule type="cellIs" dxfId="66" priority="70" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E95:G95">
+  <conditionalFormatting sqref="F97">
     <cfRule type="cellIs" dxfId="65" priority="69" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F96:G96">
+  <conditionalFormatting sqref="E97">
     <cfRule type="cellIs" dxfId="64" priority="68" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F96:G96">
+  <conditionalFormatting sqref="F98">
     <cfRule type="cellIs" dxfId="63" priority="67" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E94">
+  <conditionalFormatting sqref="F98">
     <cfRule type="cellIs" dxfId="62" priority="66" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E96">
+  <conditionalFormatting sqref="E98">
     <cfRule type="cellIs" dxfId="61" priority="65" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F97">
-    <cfRule type="cellIs" dxfId="60" priority="64" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F97">
-    <cfRule type="cellIs" dxfId="59" priority="63" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E97">
-    <cfRule type="cellIs" dxfId="58" priority="62" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F98">
-    <cfRule type="cellIs" dxfId="57" priority="61" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F98">
-    <cfRule type="cellIs" dxfId="56" priority="60" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E98">
-    <cfRule type="cellIs" dxfId="55" priority="59" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E99:E101">
+    <cfRule type="cellIs" dxfId="60" priority="59" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F101:G101 F99:F100">
+    <cfRule type="cellIs" dxfId="59" priority="61" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F101:G101 F99:F100">
+    <cfRule type="cellIs" dxfId="58" priority="60" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E102">
+    <cfRule type="cellIs" dxfId="57" priority="56" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F102:G102">
+    <cfRule type="cellIs" dxfId="56" priority="58" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F102:G102">
+    <cfRule type="cellIs" dxfId="55" priority="57" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E103">
     <cfRule type="cellIs" dxfId="54" priority="53" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F101:G101 F99:F100">
+  <conditionalFormatting sqref="F103:G103">
     <cfRule type="cellIs" dxfId="53" priority="55" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F101:G101 F99:F100">
+  <conditionalFormatting sqref="F103:G103">
     <cfRule type="cellIs" dxfId="52" priority="54" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E102">
+  <conditionalFormatting sqref="E104">
     <cfRule type="cellIs" dxfId="51" priority="50" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F102:G102">
+  <conditionalFormatting sqref="F104:G104">
     <cfRule type="cellIs" dxfId="50" priority="52" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F102:G102">
+  <conditionalFormatting sqref="F104:G104">
     <cfRule type="cellIs" dxfId="49" priority="51" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E103">
-    <cfRule type="cellIs" dxfId="48" priority="47" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F103:G103">
-    <cfRule type="cellIs" dxfId="47" priority="49" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F103:G103">
-    <cfRule type="cellIs" dxfId="46" priority="48" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E104">
-    <cfRule type="cellIs" dxfId="45" priority="44" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F104:G104">
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F104:G104">
-    <cfRule type="cellIs" dxfId="43" priority="45" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G99">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G99">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G98">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G98">
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G97">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G97">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F105:G105">
     <cfRule type="cellIs" dxfId="42" priority="43" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G99">
+  <conditionalFormatting sqref="F105:G105">
     <cfRule type="cellIs" dxfId="41" priority="42" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G98">
+  <conditionalFormatting sqref="E105">
     <cfRule type="cellIs" dxfId="40" priority="41" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G98">
+  <conditionalFormatting sqref="G100">
     <cfRule type="cellIs" dxfId="39" priority="40" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G97">
+  <conditionalFormatting sqref="G100">
     <cfRule type="cellIs" dxfId="38" priority="39" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G97">
+  <conditionalFormatting sqref="F106:G106">
     <cfRule type="cellIs" dxfId="37" priority="38" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F105:G105">
+  <conditionalFormatting sqref="F106:G106">
     <cfRule type="cellIs" dxfId="36" priority="37" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F105:G105">
+  <conditionalFormatting sqref="E106">
     <cfRule type="cellIs" dxfId="35" priority="36" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E105">
+  <conditionalFormatting sqref="F107:G107">
     <cfRule type="cellIs" dxfId="34" priority="35" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G100">
+  <conditionalFormatting sqref="F107:G107">
     <cfRule type="cellIs" dxfId="33" priority="34" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G100">
+  <conditionalFormatting sqref="E107">
     <cfRule type="cellIs" dxfId="32" priority="33" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F106:G106">
+  <conditionalFormatting sqref="F108:G108">
     <cfRule type="cellIs" dxfId="31" priority="32" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F106:G106">
+  <conditionalFormatting sqref="F108:G108">
     <cfRule type="cellIs" dxfId="30" priority="31" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E106">
+  <conditionalFormatting sqref="E108">
     <cfRule type="cellIs" dxfId="29" priority="30" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:G107">
+  <conditionalFormatting sqref="F109:G109">
     <cfRule type="cellIs" dxfId="28" priority="29" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F107:G107">
+  <conditionalFormatting sqref="F109:G109">
     <cfRule type="cellIs" dxfId="27" priority="28" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E107">
+  <conditionalFormatting sqref="E109">
     <cfRule type="cellIs" dxfId="26" priority="27" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F108:G108">
+  <conditionalFormatting sqref="F110:G110">
     <cfRule type="cellIs" dxfId="25" priority="26" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F108:G108">
+  <conditionalFormatting sqref="F110:G110">
     <cfRule type="cellIs" dxfId="24" priority="25" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E108">
+  <conditionalFormatting sqref="E110">
     <cfRule type="cellIs" dxfId="23" priority="24" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F109:G109">
+  <conditionalFormatting sqref="F111:G111">
     <cfRule type="cellIs" dxfId="22" priority="23" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F109:G109">
+  <conditionalFormatting sqref="F111:G111">
     <cfRule type="cellIs" dxfId="21" priority="22" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E109">
+  <conditionalFormatting sqref="E111">
     <cfRule type="cellIs" dxfId="20" priority="21" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F110:G110">
+  <conditionalFormatting sqref="F112:G112">
     <cfRule type="cellIs" dxfId="19" priority="20" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F110:G110">
+  <conditionalFormatting sqref="F112:G112">
     <cfRule type="cellIs" dxfId="18" priority="19" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E110">
+  <conditionalFormatting sqref="E112">
     <cfRule type="cellIs" dxfId="17" priority="18" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F111:G111">
+  <conditionalFormatting sqref="F117:G120">
     <cfRule type="cellIs" dxfId="16" priority="17" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F111:G111">
+  <conditionalFormatting sqref="F117:G120">
     <cfRule type="cellIs" dxfId="15" priority="16" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E111">
+  <conditionalFormatting sqref="E117:E120">
     <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F112:G112">
+  <conditionalFormatting sqref="F113:G116">
     <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F112:G112">
+  <conditionalFormatting sqref="F113:G116">
     <cfRule type="cellIs" dxfId="12" priority="13" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E112">
+  <conditionalFormatting sqref="E113:E116">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F117:G120">
+  <conditionalFormatting sqref="G89">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F117:G120">
+  <conditionalFormatting sqref="G89">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E117:E120">
+  <conditionalFormatting sqref="F121:G121">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F113:G116">
+  <conditionalFormatting sqref="F121:G121">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F113:G116">
+  <conditionalFormatting sqref="E121">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E113:E116">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G89">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G89">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F121:G121">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F121:G121">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E121">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="F122:G122">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F122:G122">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E122">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7358,19 +7483,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AH33"/>
+  <dimension ref="B1:AH45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="U12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="1.09765625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="3.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.09765625" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.796875" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="5.19921875" style="16" bestFit="1" customWidth="1"/>
@@ -7422,11 +7547,11 @@
       </c>
       <c r="M1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>]</v>
+        <v/>
       </c>
       <c r="N1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>]</v>
       </c>
       <c r="O1" s="26" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7645,7 +7770,7 @@
         <v>46</v>
       </c>
       <c r="C3" s="23" t="str">
-        <f>VLOOKUP(B3,Sheet1!$B$47:$C$306,2,FALSE)</f>
+        <f>VLOOKUP(B3,Sheet1!$B$47:$C$307,2,FALSE)</f>
         <v>indicatori esperenziali</v>
       </c>
       <c r="D3" s="23"/>
@@ -7685,7 +7810,7 @@
         <v>54</v>
       </c>
       <c r="C4" s="23" t="str">
-        <f>VLOOKUP(B4,Sheet1!$B$47:$C$306,2,FALSE)</f>
+        <f>VLOOKUP(B4,Sheet1!$B$47:$C$307,2,FALSE)</f>
         <v xml:space="preserve">Gestione BR Override Rosso / Arancio </v>
       </c>
       <c r="D4" s="23"/>
@@ -7729,7 +7854,7 @@
         <v>69</v>
       </c>
       <c r="C5" s="23" t="str">
-        <f>VLOOKUP(B5,Sheet1!$B$47:$C$306,2,FALSE)</f>
+        <f>VLOOKUP(B5,Sheet1!$B$47:$C$307,2,FALSE)</f>
         <v xml:space="preserve">trascinamento dello spegnimento segnale BR12 </v>
       </c>
       <c r="D5" s="23"/>
@@ -7769,7 +7894,7 @@
         <v>70</v>
       </c>
       <c r="C6" s="23" t="str">
-        <f>VLOOKUP(B6,Sheet1!$B$47:$C$306,2,FALSE)</f>
+        <f>VLOOKUP(B6,Sheet1!$B$47:$C$307,2,FALSE)</f>
         <v>override NOPG</v>
       </c>
       <c r="D6" s="23"/>
@@ -7811,7 +7936,7 @@
         <v>78</v>
       </c>
       <c r="C7" s="23" t="str">
-        <f>VLOOKUP(B7,Sheet1!$B$47:$C$306,2,FALSE)</f>
+        <f>VLOOKUP(B7,Sheet1!$B$47:$C$307,2,FALSE)</f>
         <v>override ind.36</v>
       </c>
       <c r="D7" s="23"/>
@@ -7853,7 +7978,7 @@
         <v>95</v>
       </c>
       <c r="C8" s="23" t="str">
-        <f>VLOOKUP(B8,Sheet1!$B$47:$C$306,2,FALSE)</f>
+        <f>VLOOKUP(B8,Sheet1!$B$47:$C$307,2,FALSE)</f>
         <v>override Fitch Rosso</v>
       </c>
       <c r="D8" s="23"/>
@@ -7895,7 +8020,7 @@
         <v>104</v>
       </c>
       <c r="C9" s="23" t="str">
-        <f>VLOOKUP(B9,Sheet1!$B$47:$C$306,2,FALSE)</f>
+        <f>VLOOKUP(B9,Sheet1!$B$47:$C$307,2,FALSE)</f>
         <v>override Fitch Blu chiaro</v>
       </c>
       <c r="D9" s="23"/>
@@ -7937,7 +8062,7 @@
         <v>120</v>
       </c>
       <c r="C10" s="23" t="str">
-        <f>VLOOKUP(B10,Sheet1!$B$47:$C$306,2,FALSE)</f>
+        <f>VLOOKUP(B10,Sheet1!$B$47:$C$307,2,FALSE)</f>
         <v>override NOPG colore blu chiaro</v>
       </c>
       <c r="D10" s="23"/>
@@ -7979,7 +8104,7 @@
         <v>110</v>
       </c>
       <c r="C11" s="23" t="str">
-        <f>VLOOKUP(B11,Sheet1!$B$47:$C$306,2,FALSE)</f>
+        <f>VLOOKUP(B11,Sheet1!$B$47:$C$307,2,FALSE)</f>
         <v>CR Esperienziali - nuovo indicatore e BR</v>
       </c>
       <c r="D11" s="23"/>
@@ -7994,9 +8119,11 @@
       <c r="M11" s="23"/>
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35" t="s">
+        <v>206</v>
+      </c>
       <c r="S11" s="23"/>
       <c r="T11" s="23"/>
       <c r="U11" s="23"/>
@@ -8016,27 +8143,29 @@
     </row>
     <row r="12" spans="2:34">
       <c r="B12" s="22">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="C12" s="23" t="str">
-        <f>VLOOKUP(B12,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>testare AQR per Banca BIB</v>
+        <f>VLOOKUP(B12,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>intervento correttivo XRA</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
       <c r="J12" s="23"/>
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
       <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35" t="s">
+        <v>206</v>
+      </c>
       <c r="S12" s="23"/>
       <c r="T12" s="23"/>
       <c r="U12" s="23"/>
@@ -8056,34 +8185,30 @@
     </row>
     <row r="13" spans="2:34">
       <c r="B13" s="22">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C13" s="23" t="str">
-        <f>VLOOKUP(B13,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>motore ALEX BANK</v>
+        <f>VLOOKUP(B13,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>testare AQR per Banca BIB</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29" t="s">
-        <v>255</v>
-      </c>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
       <c r="R13" s="23"/>
       <c r="S13" s="23"/>
       <c r="T13" s="23"/>
-      <c r="U13" s="29" t="s">
-        <v>207</v>
-      </c>
+      <c r="U13" s="23"/>
       <c r="V13" s="23"/>
       <c r="W13" s="23"/>
       <c r="X13" s="23"/>
@@ -8100,11 +8225,11 @@
     </row>
     <row r="14" spans="2:34">
       <c r="B14" s="22">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="23" t="str">
-        <f>VLOOKUP(B14,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>file test e TCK ALEX BANK</v>
+        <f>VLOOKUP(B14,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>motore ALEX BANK</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -8112,18 +8237,22 @@
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
       <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
       <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
+      <c r="O14" s="29" t="s">
+        <v>255</v>
+      </c>
       <c r="P14" s="29"/>
       <c r="Q14" s="29"/>
       <c r="R14" s="23"/>
       <c r="S14" s="23"/>
       <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
+      <c r="U14" s="29" t="s">
+        <v>207</v>
+      </c>
       <c r="V14" s="23"/>
       <c r="W14" s="23"/>
       <c r="X14" s="23"/>
@@ -8140,43 +8269,35 @@
     </row>
     <row r="15" spans="2:34">
       <c r="B15" s="22">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15" s="23" t="str">
-        <f>VLOOKUP(B15,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>motore CIB BANK</v>
+        <f>VLOOKUP(B15,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>file test e TCK ALEX BANK</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
-      <c r="H15" s="28"/>
+      <c r="H15" s="23"/>
       <c r="I15" s="23"/>
       <c r="J15" s="23"/>
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
-      <c r="M15" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="N15" s="23"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28" t="s">
-        <v>209</v>
-      </c>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28" t="s">
-        <v>254</v>
-      </c>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
       <c r="V15" s="23"/>
       <c r="W15" s="23"/>
       <c r="X15" s="23"/>
       <c r="Y15" s="23"/>
-      <c r="Z15" s="28" t="s">
-        <v>207</v>
-      </c>
+      <c r="Z15" s="23"/>
       <c r="AA15" s="23"/>
       <c r="AB15" s="23"/>
       <c r="AC15" s="23"/>
@@ -8188,35 +8309,43 @@
     </row>
     <row r="16" spans="2:34">
       <c r="B16" s="22">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="23" t="str">
-        <f>VLOOKUP(B16,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>file test e TCK CIB BANK</v>
+        <f>VLOOKUP(B16,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>motore CIB BANK</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
+      <c r="H16" s="28"/>
       <c r="I16" s="23"/>
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
+      <c r="M16" s="28" t="s">
+        <v>199</v>
+      </c>
       <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
+      <c r="O16" s="28"/>
       <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
+      <c r="Q16" s="28" t="s">
+        <v>209</v>
+      </c>
       <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
+      <c r="S16" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
       <c r="V16" s="23"/>
       <c r="W16" s="23"/>
       <c r="X16" s="23"/>
       <c r="Y16" s="23"/>
-      <c r="Z16" s="23"/>
+      <c r="Z16" s="28" t="s">
+        <v>207</v>
+      </c>
       <c r="AA16" s="23"/>
       <c r="AB16" s="23"/>
       <c r="AC16" s="23"/>
@@ -8228,11 +8357,11 @@
     </row>
     <row r="17" spans="2:34">
       <c r="B17" s="22">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17" s="23" t="str">
-        <f>VLOOKUP(B17,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>motore ISPRO BANK</v>
+        <f>VLOOKUP(B17,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>file test e TCK CIB BANK</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -8246,39 +8375,33 @@
       <c r="M17" s="23"/>
       <c r="N17" s="23"/>
       <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="37" t="s">
-        <v>199</v>
-      </c>
-      <c r="R17" s="23"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="37"/>
-      <c r="U17" s="37"/>
-      <c r="V17" s="37"/>
-      <c r="W17" s="37" t="s">
-        <v>254</v>
-      </c>
-      <c r="X17" s="37"/>
-      <c r="Y17" s="37"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23"/>
       <c r="Z17" s="23"/>
       <c r="AA17" s="23"/>
       <c r="AB17" s="23"/>
       <c r="AC17" s="23"/>
       <c r="AD17" s="23"/>
-      <c r="AE17" s="37" t="s">
-        <v>207</v>
-      </c>
+      <c r="AE17" s="23"/>
       <c r="AF17" s="23"/>
       <c r="AG17" s="23"/>
       <c r="AH17" s="23"/>
     </row>
     <row r="18" spans="2:34">
       <c r="B18" s="22">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" s="23" t="str">
-        <f>VLOOKUP(B18,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>file test e TCK ISPRO BANK</v>
+        <f>VLOOKUP(B18,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>motore ISPRO BANK</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -8293,32 +8416,38 @@
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
       <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
+      <c r="Q18" s="37" t="s">
+        <v>199</v>
+      </c>
       <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
+      <c r="S18" s="37"/>
       <c r="T18" s="37"/>
       <c r="U18" s="37"/>
       <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="23"/>
+      <c r="W18" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="X18" s="37"/>
+      <c r="Y18" s="37"/>
       <c r="Z18" s="23"/>
       <c r="AA18" s="23"/>
       <c r="AB18" s="23"/>
       <c r="AC18" s="23"/>
       <c r="AD18" s="23"/>
-      <c r="AE18" s="23"/>
+      <c r="AE18" s="37" t="s">
+        <v>207</v>
+      </c>
       <c r="AF18" s="23"/>
       <c r="AG18" s="23"/>
       <c r="AH18" s="23"/>
     </row>
     <row r="19" spans="2:34">
       <c r="B19" s="22">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C19" s="23" t="str">
-        <f>VLOOKUP(B19,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>Retail: costruzione file excel interno e verifica presenza Corporate</v>
+        <f>VLOOKUP(B19,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>file test e TCK ISPRO BANK</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
@@ -8328,7 +8457,7 @@
       <c r="I19" s="23"/>
       <c r="J19" s="23"/>
       <c r="K19" s="23"/>
-      <c r="L19" s="35"/>
+      <c r="L19" s="23"/>
       <c r="M19" s="23"/>
       <c r="N19" s="23"/>
       <c r="O19" s="23"/>
@@ -8336,10 +8465,10 @@
       <c r="Q19" s="23"/>
       <c r="R19" s="23"/>
       <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="37"/>
+      <c r="W19" s="37"/>
       <c r="X19" s="23"/>
       <c r="Y19" s="23"/>
       <c r="Z19" s="23"/>
@@ -8350,17 +8479,15 @@
       <c r="AE19" s="23"/>
       <c r="AF19" s="23"/>
       <c r="AG19" s="23"/>
-      <c r="AH19" s="35" t="s">
-        <v>207</v>
-      </c>
+      <c r="AH19" s="23"/>
     </row>
     <row r="20" spans="2:34">
       <c r="B20" s="22">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" s="23" t="str">
-        <f>VLOOKUP(B20,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>Retail: test di performance (2 mio di dati)</v>
+        <f>VLOOKUP(B20,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>Retail: costruzione file excel interno e verifica presenza Corporate</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -8371,7 +8498,7 @@
       <c r="J20" s="23"/>
       <c r="K20" s="23"/>
       <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
+      <c r="M20" s="23"/>
       <c r="N20" s="23"/>
       <c r="O20" s="23"/>
       <c r="P20" s="23"/>
@@ -8392,15 +8519,17 @@
       <c r="AE20" s="23"/>
       <c r="AF20" s="23"/>
       <c r="AG20" s="23"/>
-      <c r="AH20" s="23"/>
+      <c r="AH20" s="35" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="21" spans="2:34">
       <c r="B21" s="22">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C21" s="23" t="str">
-        <f>VLOOKUP(B21,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>Retail: nodo Riempimento in VM</v>
+        <f>VLOOKUP(B21,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>Retail: test di performance (2 mio di dati)</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -8410,11 +8539,11 @@
       <c r="I21" s="23"/>
       <c r="J21" s="23"/>
       <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
       <c r="N21" s="23"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
       <c r="Q21" s="23"/>
       <c r="R21" s="23"/>
       <c r="S21" s="23"/>
@@ -8436,11 +8565,11 @@
     </row>
     <row r="22" spans="2:34">
       <c r="B22" s="22">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="23" t="str">
-        <f>VLOOKUP(B22,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>Retail: sviluppo indicatori</v>
+        <f>VLOOKUP(B22,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>Retail: nodo Riempimento in VM</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -8453,23 +8582,13 @@
       <c r="L22" s="23"/>
       <c r="M22" s="23"/>
       <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="R22" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="S22" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="T22" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="U22" s="35" t="s">
-        <v>198</v>
-      </c>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
       <c r="V22" s="23"/>
       <c r="W22" s="23"/>
       <c r="X22" s="23"/>
@@ -8482,17 +8601,15 @@
       <c r="AE22" s="23"/>
       <c r="AF22" s="23"/>
       <c r="AG22" s="23"/>
-      <c r="AH22" s="35" t="s">
-        <v>207</v>
-      </c>
+      <c r="AH22" s="23"/>
     </row>
     <row r="23" spans="2:34">
       <c r="B23" s="22">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="23" t="str">
-        <f>VLOOKUP(B23,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>Retail: configurazione start-up app (excel)</v>
+        <f>VLOOKUP(B23,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>Retail: sviluppo indicatori</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
@@ -8506,13 +8623,25 @@
       <c r="M23" s="23"/>
       <c r="N23" s="23"/>
       <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
+      <c r="P23" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q23" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="R23" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="S23" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="T23" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="U23" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="V23" s="23"/>
       <c r="W23" s="23"/>
       <c r="X23" s="23"/>
       <c r="Y23" s="23"/>
@@ -8530,11 +8659,11 @@
     </row>
     <row r="24" spans="2:34">
       <c r="B24" s="22">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" s="23" t="str">
-        <f>VLOOKUP(B24,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>Retail: configurazione iniziale app e VM  (BR, Matrice e FT)</v>
+        <f>VLOOKUP(B24,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>Retail: configurazione start-up app (excel)</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
@@ -8552,11 +8681,11 @@
       <c r="Q24" s="23"/>
       <c r="R24" s="23"/>
       <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
+      <c r="T24" s="35"/>
       <c r="U24" s="35"/>
       <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
-      <c r="X24" s="35"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
       <c r="Y24" s="23"/>
       <c r="Z24" s="23"/>
       <c r="AA24" s="23"/>
@@ -8572,11 +8701,11 @@
     </row>
     <row r="25" spans="2:34">
       <c r="B25" s="22">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C25" s="23" t="str">
-        <f>VLOOKUP(B25,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>ISBA - motore</v>
+        <f>VLOOKUP(B25,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>Retail: configurazione iniziale app e VM  (BR, Matrice e FT)</v>
       </c>
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
@@ -8595,34 +8724,30 @@
       <c r="R25" s="23"/>
       <c r="S25" s="23"/>
       <c r="T25" s="23"/>
-      <c r="U25" s="23"/>
-      <c r="V25" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="W25" s="23"/>
-      <c r="X25" s="39"/>
-      <c r="Y25" s="39"/>
-      <c r="Z25" s="39"/>
-      <c r="AA25" s="39" t="s">
-        <v>254</v>
-      </c>
-      <c r="AB25" s="39"/>
-      <c r="AC25" s="39"/>
-      <c r="AD25" s="39"/>
+      <c r="U25" s="35"/>
+      <c r="V25" s="35"/>
+      <c r="W25" s="35"/>
+      <c r="X25" s="35"/>
+      <c r="Y25" s="23"/>
+      <c r="Z25" s="23"/>
+      <c r="AA25" s="23"/>
+      <c r="AB25" s="23"/>
+      <c r="AC25" s="23"/>
+      <c r="AD25" s="23"/>
       <c r="AE25" s="23"/>
       <c r="AF25" s="23"/>
       <c r="AG25" s="23"/>
-      <c r="AH25" s="39" t="s">
+      <c r="AH25" s="35" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="26" spans="2:34">
       <c r="B26" s="22">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26" s="23" t="str">
-        <f>VLOOKUP(B26,Sheet1!$B$47:$C$306,2,FALSE)</f>
-        <v>ISBA - file test e TCK</v>
+        <f>VLOOKUP(B26,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>ISBA - motore</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
@@ -8642,54 +8767,164 @@
       <c r="S26" s="23"/>
       <c r="T26" s="23"/>
       <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
+      <c r="V26" s="39" t="s">
+        <v>199</v>
+      </c>
       <c r="W26" s="23"/>
-      <c r="X26" s="23"/>
+      <c r="X26" s="39"/>
       <c r="Y26" s="39"/>
       <c r="Z26" s="39"/>
-      <c r="AA26" s="39"/>
+      <c r="AA26" s="39" t="s">
+        <v>254</v>
+      </c>
       <c r="AB26" s="39"/>
-      <c r="AC26" s="23"/>
-      <c r="AD26" s="23"/>
+      <c r="AC26" s="39"/>
+      <c r="AD26" s="39"/>
       <c r="AE26" s="23"/>
       <c r="AF26" s="23"/>
       <c r="AG26" s="23"/>
-      <c r="AH26" s="23"/>
-    </row>
-    <row r="28" spans="2:34">
-      <c r="B28" s="35"/>
-      <c r="C28" s="16" t="s">
+      <c r="AH26" s="39" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="2:34">
+      <c r="B27" s="22">
+        <v>118</v>
+      </c>
+      <c r="C27" s="23" t="str">
+        <f>VLOOKUP(B27,Sheet1!$B$47:$C$307,2,FALSE)</f>
+        <v>ISBA - file test e TCK</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="39"/>
+      <c r="Z27" s="39"/>
+      <c r="AA27" s="39"/>
+      <c r="AB27" s="39"/>
+      <c r="AC27" s="23"/>
+      <c r="AD27" s="23"/>
+      <c r="AE27" s="23"/>
+      <c r="AF27" s="23"/>
+      <c r="AG27" s="23"/>
+      <c r="AH27" s="23"/>
+    </row>
+    <row r="29" spans="2:34">
+      <c r="B29" s="35"/>
+      <c r="C29" s="16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="2:34">
-      <c r="B29" s="24"/>
-      <c r="C29" s="16" t="s">
+    <row r="30" spans="2:34">
+      <c r="B30" s="24"/>
+      <c r="C30" s="16" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="2:34">
-      <c r="B30" s="25"/>
-      <c r="C30" s="16" t="s">
+    <row r="31" spans="2:34">
+      <c r="B31" s="25"/>
+      <c r="C31" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="2:34">
-      <c r="B31" s="27"/>
-      <c r="C31" s="16" t="s">
+    <row r="32" spans="2:34">
+      <c r="B32" s="27"/>
+      <c r="C32" s="16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="2:34">
-      <c r="B32" s="36"/>
-      <c r="C32" s="16" t="s">
+    <row r="33" spans="2:3">
+      <c r="B33" s="36"/>
+      <c r="C33" s="16" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
-      <c r="B33" s="30"/>
-      <c r="C33" s="16" t="s">
+    <row r="34" spans="2:3">
+      <c r="B34" s="30"/>
+      <c r="C34" s="16" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="61">
+        <v>42782</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="61">
+        <v>42786</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="61">
+        <v>42790</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="61">
+        <v>42786</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" s="61">
+        <v>42796</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" s="61">
+        <v>42797</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" s="61">
+        <v>42802</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" s="61">
+        <v>42803</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -8707,7 +8942,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.8"/>
@@ -8718,10 +8953,10 @@
     <col min="4" max="5" width="6.09765625" style="16" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="5.796875" style="16" customWidth="1"/>
     <col min="7" max="7" width="7.3984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.796875" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.796875" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.796875" style="16" customWidth="1"/>
-    <col min="11" max="25" width="5.796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="25" width="5.796875" style="16" bestFit="1" customWidth="1"/>
     <col min="26" max="48" width="6.19921875" style="16" bestFit="1" customWidth="1"/>
     <col min="49" max="68" width="5.796875" style="16" bestFit="1" customWidth="1"/>
     <col min="69" max="91" width="6.5" style="16" bestFit="1" customWidth="1"/>
@@ -8757,7 +8992,7 @@
       </c>
       <c r="H1" s="26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>]</v>
+        <v/>
       </c>
       <c r="I1" s="26" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -8765,7 +9000,7 @@
       </c>
       <c r="J1" s="26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>]</v>
       </c>
       <c r="K1" s="26" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -9705,11 +9940,11 @@
         <v>231</v>
       </c>
       <c r="H3" s="47"/>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="48" t="s">
         <v>231</v>
       </c>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
       <c r="L3" s="47"/>
       <c r="M3" s="47"/>
       <c r="N3" s="49"/>

</xml_diff>